<commit_message>
updated scripts and added new scripts
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aef5f9141681d0eb/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A881168C-430E-46BD-8843-5EE800A5922F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{43F4365A-3698-4E21-8DAD-CAC7092D65C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="2568" windowWidth="17280" windowHeight="8964" xr2:uid="{28CACC02-7B62-4E4B-9E75-F1D3B1075A05}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="17340" windowHeight="11820" xr2:uid="{28CACC02-7B62-4E4B-9E75-F1D3B1075A05}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
     <sheet name="deals" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,54 +23,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>company</t>
   </si>
   <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Cris</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Alagu</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
     <t>Mr.</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
     <t>Dr.</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Cris</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
     <t>Mrs.</t>
-  </si>
-  <si>
-    <t>Raja</t>
-  </si>
-  <si>
-    <t>Alagu</t>
-  </si>
-  <si>
-    <t>Ebay</t>
   </si>
 </sst>
 </file>
@@ -458,64 +451,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D348007A-FBB8-49C5-9C01-4D6594202DAF}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -544,7 +539,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>